<commit_message>
Didier's updates (part 1)
</commit_message>
<xml_diff>
--- a/agquery/Update/grouping_vars.xlsx
+++ b/agquery/Update/grouping_vars.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altomes\Desktop\50x30_AQP\agquery\Update\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\R\50x30AQP\agquery\Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB68819-F797-4937-AA7C-17B678F0AA42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87DF53C8-FF0B-4FDC-A340-5E4FA7038EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="3855" windowWidth="29010" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2415" yWindow="750" windowWidth="23175" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -105,7 +105,7 @@
     <t>Household</t>
   </si>
   <si>
-    <t>Household &lt;font style = 'font-weight:normal'&gt;&lt;i&gt;(Optional)&lt;/font&gt;&lt;/i&gt;</t>
+    <t>Disaggregates</t>
   </si>
 </sst>
 </file>
@@ -426,7 +426,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD8"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updates to interface layout and fixed a bug where the chart wasn't displaying for household
</commit_message>
<xml_diff>
--- a/agquery/Update/grouping_vars.xlsx
+++ b/agquery/Update/grouping_vars.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altomes\Desktop\50x30_AQP\agquery\Update\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\R\50x30AQP\agquery\Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104754D7-4780-45BD-88F3-64D1202AEA9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E372D653-B624-42F0-9F69-802FA3C487A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42330" yWindow="1515" windowWidth="23355" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>varName</t>
   </si>
@@ -438,7 +438,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,6 +550,9 @@
       <c r="G4" t="s">
         <v>18</v>
       </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">

</xml_diff>

<commit_message>
Edits to RShiny interface
</commit_message>
<xml_diff>
--- a/agquery/Update/grouping_vars.xlsx
+++ b/agquery/Update/grouping_vars.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\R\50x30AQP\agquery\Update\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Project\EPAR\Working Files\RA Working Folders\Sam\50x30_AQP\agquery\Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E372D653-B624-42F0-9F69-802FA3C487A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E411F8DB-B2C2-46C1-979A-61DE04EE5CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,9 +84,6 @@
     <t>Household</t>
   </si>
   <si>
-    <t>Disaggregates</t>
-  </si>
-  <si>
     <t>livestock_area</t>
   </si>
   <si>
@@ -118,6 +115,9 @@
   </si>
   <si>
     <t>Association Membership</t>
+  </si>
+  <si>
+    <t>Select Disaggregates</t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H3" sqref="H3:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,67 +499,67 @@
         <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>24</v>
       </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>25</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>26</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
       </c>
       <c r="G3" t="s">
         <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>29</v>
       </c>
-      <c r="C4" t="s">
-        <v>30</v>
-      </c>
       <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
         <v>25</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>27</v>
       </c>
       <c r="G4" t="s">
         <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -577,7 +577,7 @@
         <v>18</v>
       </c>
       <c r="H5" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final update before public release for Feb meeting
</commit_message>
<xml_diff>
--- a/agquery/Update/grouping_vars.xlsx
+++ b/agquery/Update/grouping_vars.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Project\EPAR\Working Files\RA Working Folders\Sam\50x30_AQP\agquery\Update\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altomes\Desktop\50x30_AQP\agquery\Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E411F8DB-B2C2-46C1-979A-61DE04EE5CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2ED1039-9121-42B6-9AEA-8C675EC96911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,15 +51,9 @@
     <t>Gender of Household Head</t>
   </si>
   <si>
-    <t>Farm Size</t>
-  </si>
-  <si>
     <t>As labeled</t>
   </si>
   <si>
-    <t>Male/Female Household Head</t>
-  </si>
-  <si>
     <t>Levels</t>
   </si>
   <si>
@@ -118,6 +112,12 @@
   </si>
   <si>
     <t>Select Disaggregates</t>
+  </si>
+  <si>
+    <t>Livestock Area</t>
+  </si>
+  <si>
+    <t>Household Head Gender</t>
   </si>
 </sst>
 </file>
@@ -438,13 +438,13 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:H5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="18.42578125" customWidth="1"/>
     <col min="6" max="6" width="28.85546875" bestFit="1" customWidth="1"/>
@@ -461,10 +461,10 @@
         <v>5</v>
       </c>
       <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
         <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -473,7 +473,7 @@
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -484,100 +484,100 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
       </c>
       <c r="F2" t="s">
         <v>4</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>24</v>
       </c>
-      <c r="E3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" t="s">
-        <v>26</v>
-      </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
         <v>28</v>
-      </c>
-      <c r="C4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>16</v>
       </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
-      </c>
       <c r="H5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Major update to incorporate 2021 CAS data (in progress)
</commit_message>
<xml_diff>
--- a/agquery/Update/grouping_vars.xlsx
+++ b/agquery/Update/grouping_vars.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\R\50x30AQP\agquery\Update\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altomes\Desktop\50x30_AQP\agquery\Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E372D653-B624-42F0-9F69-802FA3C487A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C0631D-CB23-404A-89A6-05CFCCE591C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>varName</t>
   </si>
@@ -36,12 +36,6 @@
     <t>fhh</t>
   </si>
   <si>
-    <t>definition</t>
-  </si>
-  <si>
-    <t>1 = household has female head</t>
-  </si>
-  <si>
     <t>shortName</t>
   </si>
   <si>
@@ -54,9 +48,6 @@
     <t>Farm Size</t>
   </si>
   <si>
-    <t>As labeled</t>
-  </si>
-  <si>
     <t>Male/Female Household Head</t>
   </si>
   <si>
@@ -78,15 +69,6 @@
     <t>0 ha,&gt;0-2 ha,&gt;2-4 ha,&gt;4 ha</t>
   </si>
   <si>
-    <t>level_lab</t>
-  </si>
-  <si>
-    <t>Household</t>
-  </si>
-  <si>
-    <t>Disaggregates</t>
-  </si>
-  <si>
     <t>livestock_area</t>
   </si>
   <si>
@@ -108,9 +90,6 @@
     <t>Yes,No</t>
   </si>
   <si>
-    <t>1=Yes, 2=No</t>
-  </si>
-  <si>
     <t>ag_comm</t>
   </si>
   <si>
@@ -118,6 +97,72 @@
   </si>
   <si>
     <t>Association Membership</t>
+  </si>
+  <si>
+    <t>feed_Chickens</t>
+  </si>
+  <si>
+    <t>Chicken Feeding Practice</t>
+  </si>
+  <si>
+    <t>Type of Feed</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>Only Grazing,Mixed,Only Feed</t>
+  </si>
+  <si>
+    <t>Poultry</t>
+  </si>
+  <si>
+    <t>drought</t>
+  </si>
+  <si>
+    <t>flood</t>
+  </si>
+  <si>
+    <t>irrigation</t>
+  </si>
+  <si>
+    <t>Household Experienced Drought</t>
+  </si>
+  <si>
+    <t>Household Experienced Flood</t>
+  </si>
+  <si>
+    <t>Household Used Irrigation</t>
+  </si>
+  <si>
+    <t>Drought</t>
+  </si>
+  <si>
+    <t>Flooding</t>
+  </si>
+  <si>
+    <t>Irrigation Use</t>
+  </si>
+  <si>
+    <t>No Drought,Drought</t>
+  </si>
+  <si>
+    <t>No Flooding,Flooding</t>
+  </si>
+  <si>
+    <t>No Irrigation,Irrigation</t>
+  </si>
+  <si>
+    <t>feed_Cattle</t>
+  </si>
+  <si>
+    <t>Livestock Feeding Practice</t>
+  </si>
+  <si>
+    <t>Livestock</t>
   </si>
 </sst>
 </file>
@@ -435,149 +480,218 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="28.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="H2" t="s">
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
         <v>27</v>
       </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
         <v>27</v>
       </c>
-      <c r="G4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" t="s">
-        <v>19</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to app in progress; still need to fix getData function
</commit_message>
<xml_diff>
--- a/agquery/Update/grouping_vars.xlsx
+++ b/agquery/Update/grouping_vars.xlsx
@@ -5,27 +5,38 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altomes\Desktop\50x30_AQP\agquery\Update\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skenne3\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551940AD-8631-4CE3-934C-3DF17811DB54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4DA7C6-B326-42AA-A086-CC2E864F7F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38220" yWindow="1635" windowWidth="23355" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
   <si>
     <t>varName</t>
   </si>
@@ -148,6 +159,33 @@
   </si>
   <si>
     <t>Livestock</t>
+  </si>
+  <si>
+    <t>rice</t>
+  </si>
+  <si>
+    <t>extension_training</t>
+  </si>
+  <si>
+    <t>Household cultivated rice</t>
+  </si>
+  <si>
+    <t>Rice</t>
+  </si>
+  <si>
+    <t>Extension Training</t>
+  </si>
+  <si>
+    <t>Household Received Extension Training</t>
+  </si>
+  <si>
+    <t>Household dedicated space to livestock</t>
+  </si>
+  <si>
+    <t>Dedicated Livestock Area</t>
+  </si>
+  <si>
+    <t>animal_ded_area</t>
   </si>
 </sst>
 </file>
@@ -465,17 +503,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -659,6 +697,66 @@
         <v>40</v>
       </c>
     </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>